<commit_message>
Se modificó el modelo de los motores, se le añadió el factor Bm en la función de transferencia
</commit_message>
<xml_diff>
--- a/Motores/Modelado/Calculos.xlsx
+++ b/Motores/Modelado/Calculos.xlsx
@@ -22,7 +22,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">v/b</t>
+  </si>
   <si>
     <t xml:space="preserve">M2</t>
   </si>
@@ -64,6 +67,18 @@
   </si>
   <si>
     <t xml:space="preserve">k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r/n</t>
   </si>
   <si>
     <t xml:space="preserve">M1</t>
@@ -260,7 +275,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -369,11 +384,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="94704617"/>
-        <c:axId val="53419375"/>
+        <c:axId val="57032488"/>
+        <c:axId val="78009749"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94704617"/>
+        <c:axId val="57032488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -409,12 +424,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53419375"/>
+        <c:crossAx val="78009749"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53419375"/>
+        <c:axId val="78009749"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -450,7 +465,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94704617"/>
+        <c:crossAx val="57032488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -477,7 +492,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -532,7 +547,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$22:$D$26</c:f>
+              <c:f>Sheet1!$D$24:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -556,7 +571,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$22:$C$26</c:f>
+              <c:f>Sheet1!$C$24:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -580,11 +595,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="59219304"/>
-        <c:axId val="76567582"/>
+        <c:axId val="33851870"/>
+        <c:axId val="24978126"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59219304"/>
+        <c:axId val="33851870"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,12 +635,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76567582"/>
+        <c:crossAx val="24978126"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76567582"/>
+        <c:axId val="24978126"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +676,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59219304"/>
+        <c:crossAx val="33851870"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -693,7 +708,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:colOff>320400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>76320</xdr:rowOff>
     </xdr:from>
@@ -709,8 +724,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5044320" y="76320"/>
-        <a:ext cx="2888280" cy="2041560"/>
+        <a:off x="5269320" y="76320"/>
+        <a:ext cx="2840400" cy="2041560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -723,15 +738,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>312480</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:colOff>312840</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>159480</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -739,8 +754,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5036760" y="3840480"/>
-        <a:ext cx="3390120" cy="2205360"/>
+        <a:off x="5261760" y="4191120"/>
+        <a:ext cx="3332880" cy="2205000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -758,36 +773,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C1:Q37"/>
+  <dimension ref="B1:Q43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="16" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5"/>
+    <col collapsed="false" hidden="false" max="16" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,7 +818,7 @@
         <v>0.58</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2" t="n">
         <f aca="false" t="array" ref="F3:G6">LINEST(C3:C8,D3:D8,0,1)</f>
@@ -808,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="3" t="n">
         <v>1.93082E-005</v>
@@ -874,15 +894,15 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,7 +915,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
@@ -903,7 +923,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>26</v>
@@ -912,7 +932,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="4" t="n">
         <f aca="false">D13/D12</f>
@@ -922,7 +942,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2.7227</v>
@@ -931,7 +951,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="4" t="n">
         <f aca="false">C11-F3*D11</f>
@@ -941,7 +961,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D17" s="4" t="n">
         <f aca="false">D16/D15</f>
@@ -950,171 +970,231 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="4"/>
+      <c r="C19" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>1.93082E-005</v>
+      </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <f aca="false">((1/D21)-D17^2)/F3</f>
+        <v>0.186442462912326</v>
+      </c>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>3.478</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="0" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="0" t="n">
+      <c r="D23" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D24" s="0" t="n">
         <v>0.35</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2" t="n">
-        <f aca="false" t="array" ref="F22:G25">LINEST(C22:C26,D22:D26,0,1)</f>
+      <c r="E24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <f aca="false" t="array" ref="F24:G27">LINEST(C24:C28,D24:D28,0,1)</f>
         <v>1.11337030811197</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G24" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H22" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0" t="n">
+      <c r="H24" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D25" s="0" t="n">
         <v>0.83</v>
       </c>
-      <c r="F23" s="4" t="n">
+      <c r="F25" s="4" t="n">
         <v>0.0250875554057343</v>
       </c>
-      <c r="G23" s="0" t="str">
+      <c r="G25" s="0" t="str">
         <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>0.997973174880593</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <v>0.0790743668540678</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>1.82</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>1969.52991222528</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0.997973174880593</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0.0790743668540678</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>1969.52991222528</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0" t="n">
         <v>2.2</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D28" s="0" t="n">
         <v>2.03</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D32" s="0" t="n">
         <v>0.17</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="0" t="n">
-        <v>27</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="4" t="n">
-        <f aca="false">D33/D32</f>
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="4" t="n">
-        <v>2.827</v>
+        <v>10</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36" s="4" t="n">
-        <f aca="false">ABS(C30-F22*D30)</f>
-        <v>0.810727047620965</v>
+        <f aca="false">D35/D34</f>
+        <v>27</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="4" t="n">
+        <v>2.827</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="4" t="n">
-        <f aca="false">D36/D35</f>
+      <c r="D38" s="4" t="n">
+        <f aca="false">ABS(C32-F24*D32)</f>
+        <v>0.810727047620965</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="4" t="n">
+        <f aca="false">D38/D37</f>
         <v>0.286779995621141</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>1.93082E-005</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <f aca="false">((1/D43)-D39^2)/F25</f>
+        <v>8.18249506215046</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>3.478</v>
       </c>
     </row>
   </sheetData>
@@ -1137,12 +1217,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C42:D43 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1163,12 +1243,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C42:D43 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Se añaden imagenes para la wiki
</commit_message>
<xml_diff>
--- a/Motores/Modelado/Calculos.xlsx
+++ b/Motores/Modelado/Calculos.xlsx
@@ -275,7 +275,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -384,11 +384,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="57032488"/>
-        <c:axId val="78009749"/>
+        <c:axId val="92129716"/>
+        <c:axId val="98611368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57032488"/>
+        <c:axId val="92129716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -424,12 +424,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78009749"/>
+        <c:crossAx val="98611368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78009749"/>
+        <c:axId val="98611368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,7 +465,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57032488"/>
+        <c:crossAx val="92129716"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -492,7 +492,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -595,11 +595,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="33851870"/>
-        <c:axId val="24978126"/>
+        <c:axId val="34627444"/>
+        <c:axId val="11993418"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33851870"/>
+        <c:axId val="34627444"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,12 +635,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24978126"/>
+        <c:crossAx val="11993418"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="24978126"/>
+        <c:axId val="11993418"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +676,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33851870"/>
+        <c:crossAx val="34627444"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -776,7 +776,7 @@
   <dimension ref="B1:Q43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42:D43"/>
+      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -990,8 +990,8 @@
         <v>16</v>
       </c>
       <c r="D20" s="3" t="n">
-        <f aca="false">((1/D21)-D17^2)/F3</f>
-        <v>0.186442462912326</v>
+        <f aca="false">(D17/D21)-D17^2</f>
+        <v>-0.00114843859360879</v>
       </c>
       <c r="F20" s="4"/>
     </row>
@@ -1185,8 +1185,8 @@
         <v>16</v>
       </c>
       <c r="D42" s="3" t="n">
-        <f aca="false">((1/D43)-D39^2)/F25</f>
-        <v>8.18249506215046</v>
+        <f aca="false">((D39/D43)-D39^2)/F24</f>
+        <v>0.000191011928856257</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,7 +1217,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C42:D43 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1243,7 +1243,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C42:D43 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Se añadieron las imágenes correspondientes al resultado de la simulacion del motor
</commit_message>
<xml_diff>
--- a/Motores/Modelado/Calculos.xlsx
+++ b/Motores/Modelado/Calculos.xlsx
@@ -275,7 +275,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -384,11 +384,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="92129716"/>
-        <c:axId val="98611368"/>
+        <c:axId val="22710332"/>
+        <c:axId val="24990759"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92129716"/>
+        <c:axId val="22710332"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -424,12 +424,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98611368"/>
+        <c:crossAx val="24990759"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98611368"/>
+        <c:axId val="24990759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,7 +465,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92129716"/>
+        <c:crossAx val="22710332"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -492,7 +492,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -595,11 +595,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="34627444"/>
-        <c:axId val="11993418"/>
+        <c:axId val="13410107"/>
+        <c:axId val="58599180"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34627444"/>
+        <c:axId val="13410107"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,12 +635,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11993418"/>
+        <c:crossAx val="58599180"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="11993418"/>
+        <c:axId val="58599180"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +676,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34627444"/>
+        <c:crossAx val="13410107"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -714,9 +714,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>255600</xdr:colOff>
+      <xdr:colOff>255240</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -724,8 +724,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5269320" y="76320"/>
-        <a:ext cx="2840400" cy="2041560"/>
+        <a:off x="5187600" y="76320"/>
+        <a:ext cx="2792160" cy="2041200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -744,9 +744,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>159480</xdr:colOff>
+      <xdr:colOff>159120</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -754,8 +754,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5261760" y="4191120"/>
-        <a:ext cx="3332880" cy="2205000"/>
+        <a:off x="5180040" y="4191120"/>
+        <a:ext cx="3275280" cy="2204640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -776,16 +776,16 @@
   <dimension ref="B1:Q43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5"/>
-    <col collapsed="false" hidden="false" max="16" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="5" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,7 +973,9 @@
       <c r="C18" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="4" t="n">
+        <v>0.000336</v>
+      </c>
       <c r="F18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,6 +1172,9 @@
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>0.000286</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,7 +1227,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1248,7 +1253,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>